<commit_message>
language and final results
</commit_message>
<xml_diff>
--- a/src/language.xlsx
+++ b/src/language.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kawczakr\Downloads\git\Dices\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Radek\Desktop\coding\Dices\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F681BFC9-C312-4870-9FB9-E4C2C70B8BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09F7F83-DE57-4957-A10E-FF2C44416511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3876" yWindow="504" windowWidth="17280" windowHeight="8964" xr2:uid="{B56B30AD-E1F9-4485-9E65-621CFB902A1D}"/>
+    <workbookView xWindow="-25260" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{B56B30AD-E1F9-4485-9E65-621CFB902A1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -499,14 +499,14 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -517,7 +517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -528,7 +528,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -539,7 +539,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -550,7 +550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -561,7 +561,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -572,7 +572,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -583,7 +583,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -594,7 +594,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -605,7 +605,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -616,7 +616,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -627,7 +627,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>

</xml_diff>